<commit_message>
Work done till 01-08-2017
</commit_message>
<xml_diff>
--- a/api/MIS Reports/Analysis Lot Files/analysis printing_winer_2016_Lot-4.xlsx
+++ b/api/MIS Reports/Analysis Lot Files/analysis printing_winer_2016_Lot-4.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="78">
   <si>
     <t>Sr.No.</t>
   </si>
@@ -261,30 +261,6 @@
   </si>
   <si>
     <t>Ahmedabad</t>
-  </si>
-  <si>
-    <t>Columbia Convent School</t>
-  </si>
-  <si>
-    <t>Indore</t>
-  </si>
-  <si>
-    <t>Delhi Public School</t>
-  </si>
-  <si>
-    <t>Ryan International School, Nerul</t>
-  </si>
-  <si>
-    <t>Sri Shenbaga Vinayagar Matriculation Higher Secondary School</t>
-  </si>
-  <si>
-    <t>Sivakasi</t>
-  </si>
-  <si>
-    <t>St. Joseph^s High School, CBSE</t>
-  </si>
-  <si>
-    <t>New Panvel</t>
   </si>
 </sst>
 </file>
@@ -1145,10 +1121,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V40"/>
+  <dimension ref="A1:V35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3312,319 +3288,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A36" s="1">
-        <v>35</v>
-      </c>
-      <c r="B36" s="1">
-        <v>89386</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E36" s="1">
-        <v>867</v>
-      </c>
-      <c r="F36" s="1">
-        <v>867</v>
-      </c>
-      <c r="G36" s="1">
-        <v>23312</v>
-      </c>
-      <c r="H36" s="1">
-        <v>867</v>
-      </c>
-      <c r="I36" s="1">
-        <v>75</v>
-      </c>
-      <c r="J36" s="1">
-        <v>1512</v>
-      </c>
-      <c r="K36" s="1">
-        <v>0</v>
-      </c>
-      <c r="L36" s="1">
-        <v>0</v>
-      </c>
-      <c r="M36" s="1">
-        <v>0</v>
-      </c>
-      <c r="N36" s="1">
-        <v>0</v>
-      </c>
-      <c r="O36" s="1">
-        <v>0</v>
-      </c>
-      <c r="P36" s="1">
-        <v>78</v>
-      </c>
-      <c r="Q36" s="1">
-        <v>26</v>
-      </c>
-      <c r="R36" s="1">
-        <v>4</v>
-      </c>
-      <c r="S36" s="1">
-        <v>58</v>
-      </c>
-      <c r="T36" s="1">
-        <v>64</v>
-      </c>
-      <c r="U36" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A37" s="1">
-        <v>36</v>
-      </c>
-      <c r="B37" s="1">
-        <v>3293950</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E37" s="1">
-        <v>42</v>
-      </c>
-      <c r="F37" s="1">
-        <v>42</v>
-      </c>
-      <c r="G37" s="1">
-        <v>760</v>
-      </c>
-      <c r="H37" s="1">
-        <v>42</v>
-      </c>
-      <c r="I37" s="1">
-        <v>0</v>
-      </c>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1">
-        <v>0</v>
-      </c>
-      <c r="L37" s="1">
-        <v>0</v>
-      </c>
-      <c r="M37" s="1">
-        <v>0</v>
-      </c>
-      <c r="N37" s="1">
-        <v>0</v>
-      </c>
-      <c r="O37" s="1">
-        <v>0</v>
-      </c>
-      <c r="P37" s="1">
-        <v>23</v>
-      </c>
-      <c r="Q37" s="1">
-        <v>9</v>
-      </c>
-      <c r="R37" s="1">
-        <v>1</v>
-      </c>
-      <c r="S37" s="1">
-        <v>12</v>
-      </c>
-      <c r="T37" s="1">
-        <v>16</v>
-      </c>
-      <c r="U37" s="1"/>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A38" s="1">
-        <v>37</v>
-      </c>
-      <c r="B38" s="1">
-        <v>374289</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E38" s="1">
-        <v>28</v>
-      </c>
-      <c r="F38" s="1">
-        <v>28</v>
-      </c>
-      <c r="G38" s="1">
-        <v>512</v>
-      </c>
-      <c r="H38" s="1">
-        <v>28</v>
-      </c>
-      <c r="I38" s="1">
-        <v>0</v>
-      </c>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1">
-        <v>1</v>
-      </c>
-      <c r="L38" s="1">
-        <v>0</v>
-      </c>
-      <c r="M38" s="1">
-        <v>0</v>
-      </c>
-      <c r="N38" s="1">
-        <v>0</v>
-      </c>
-      <c r="O38" s="1">
-        <v>0</v>
-      </c>
-      <c r="P38" s="1">
-        <v>35</v>
-      </c>
-      <c r="Q38" s="1">
-        <v>17</v>
-      </c>
-      <c r="R38" s="1">
-        <v>1</v>
-      </c>
-      <c r="S38" s="1">
-        <v>12</v>
-      </c>
-      <c r="T38" s="1">
-        <v>28</v>
-      </c>
-      <c r="U38" s="1"/>
-    </row>
-    <row r="39" spans="1:21" ht="30" x14ac:dyDescent="0.2">
-      <c r="A39" s="1">
-        <v>38</v>
-      </c>
-      <c r="B39" s="1">
-        <v>1596332</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E39" s="1">
-        <v>277</v>
-      </c>
-      <c r="F39" s="1">
-        <v>277</v>
-      </c>
-      <c r="G39" s="1">
-        <v>7668</v>
-      </c>
-      <c r="H39" s="1">
-        <v>277</v>
-      </c>
-      <c r="I39" s="1">
-        <v>21</v>
-      </c>
-      <c r="J39" s="1">
-        <v>436</v>
-      </c>
-      <c r="K39" s="1">
-        <v>0</v>
-      </c>
-      <c r="L39" s="1">
-        <v>0</v>
-      </c>
-      <c r="M39" s="1">
-        <v>0</v>
-      </c>
-      <c r="N39" s="1">
-        <v>0</v>
-      </c>
-      <c r="O39" s="1">
-        <v>0</v>
-      </c>
-      <c r="P39" s="1">
-        <v>24</v>
-      </c>
-      <c r="Q39" s="1">
-        <v>8</v>
-      </c>
-      <c r="R39" s="1">
-        <v>2</v>
-      </c>
-      <c r="S39" s="1">
-        <v>24</v>
-      </c>
-      <c r="T39" s="1">
-        <v>28</v>
-      </c>
-      <c r="U39" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A40" s="1">
-        <v>39</v>
-      </c>
-      <c r="B40" s="1">
-        <v>389255</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E40" s="1">
-        <v>31</v>
-      </c>
-      <c r="F40" s="1">
-        <v>31</v>
-      </c>
-      <c r="G40" s="1">
-        <v>500</v>
-      </c>
-      <c r="H40" s="1">
-        <v>31</v>
-      </c>
-      <c r="I40" s="1">
-        <v>0</v>
-      </c>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1">
-        <v>0</v>
-      </c>
-      <c r="L40" s="1">
-        <v>0</v>
-      </c>
-      <c r="M40" s="1">
-        <v>0</v>
-      </c>
-      <c r="N40" s="1">
-        <v>0</v>
-      </c>
-      <c r="O40" s="1">
-        <v>0</v>
-      </c>
-      <c r="P40" s="1">
-        <v>28</v>
-      </c>
-      <c r="Q40" s="1">
-        <v>16</v>
-      </c>
-      <c r="R40" s="1">
-        <v>3</v>
-      </c>
-      <c r="S40" s="1">
-        <v>6</v>
-      </c>
-      <c r="T40" s="1">
-        <v>22</v>
-      </c>
-      <c r="U40" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>